<commit_message>
Support scaling factor wildcards for GNFR and emission type
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/02_scaling/scaling.xlsx
+++ b/logic/test/data/_input/02_scaling/scaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\_input\02_scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8EF75F-AF42-4105-8278-8BAAC47EE59C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CB0CE2-7CD4-46D6-814C-CF858DBDDD7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="6" xr2:uid="{6C3FE3BB-8C73-4241-95BD-F737EA4A19F7}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="447">
   <si>
     <t>A_PublicPower</t>
   </si>
@@ -1535,27 +1535,7 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="17">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1853,51 +1833,51 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6617CD5-2290-43AE-9640-6C7136C3D81F}" name="tbl_I_scaling" displayName="tbl_I_scaling" ref="A1:S8" totalsRowShown="0">
-  <autoFilter ref="A1:S8" xr:uid="{63E30767-0150-412D-B197-11CE9D14EB4E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6617CD5-2290-43AE-9640-6C7136C3D81F}" name="tbl_I_scaling" displayName="tbl_I_scaling" ref="A1:S9" totalsRowShown="0">
+  <autoFilter ref="A1:S9" xr:uid="{63E30767-0150-412D-B197-11CE9D14EB4E}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{3CCF1BDF-57B8-4181-91EA-C6A954F57C6F}" name="year" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{3CCF1BDF-57B8-4181-91EA-C6A954F57C6F}" name="year" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{85345B25-FBFE-4C64-BB97-93F81600465B}" name="emission_type"/>
     <tableColumn id="3" xr3:uid="{E47F6DBE-843D-4D02-9E5B-FEE4182373E7}" name="pollutant_code"/>
     <tableColumn id="8" xr3:uid="{E38CAB6A-CB47-4542-997D-36BA98FB4911}" name="country_iso_code"/>
     <tableColumn id="4" xr3:uid="{98A5C858-28E9-44AB-8218-0A98439E4FDD}" name="GNFR_code"/>
     <tableColumn id="5" xr3:uid="{E012C600-87B4-47D1-9988-30D2C112D83D}" name="NFR_code"/>
     <tableColumn id="12" xr3:uid="{2155F8C1-A823-4717-B464-22F4A9A05E6A}" name="scale_factor"/>
-    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="13">
       <calculatedColumnFormula>INDEX(tbl_country[country_label],MATCH(tbl_I_scaling[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="14">
+    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="12">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="13">
+    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="11">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="12">
+    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="11">
+    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="9">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="10">
+    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="8">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{F0E4C9D2-7F88-4B77-907E-74002F493346}" name="E-MAP_emission_type" dataDxfId="9">
+    <tableColumn id="14" xr3:uid="{F0E4C9D2-7F88-4B77-907E-74002F493346}" name="E-MAP_emission_type" dataDxfId="7">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[emission_type]]),"",tbl_I_scaling[[#This Row],[emission_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="8">
+    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[pollutant_code]]),"",tbl_I_scaling[[#This Row],[pollutant_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="7">
+    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[country_iso_code]]),"",tbl_I_scaling[[#This Row],[country_iso_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="6">
+    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_scaling[[#This Row],[GNFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="5">
+    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="3">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[NFR_code]]),"*",tbl_I_scaling[[#This Row],[NFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_scale_factor" dataDxfId="4">
+    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_scale_factor" dataDxfId="2">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[scale_factor]]),"",tbl_I_scaling[[#This Row],[scale_factor]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5021,10 +5001,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5575,29 +5555,98 @@
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>2005</v>
+      </c>
+      <c r="B9" t="s">
+        <v>444</v>
+      </c>
+      <c r="C9" t="s">
+        <v>407</v>
+      </c>
+      <c r="D9" t="s">
+        <v>369</v>
+      </c>
+      <c r="E9" t="s">
+        <v>444</v>
+      </c>
+      <c r="G9">
+        <v>0.8</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f>INDEX(tbl_country[country_label],MATCH(tbl_I_scaling[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</f>
+        <v>Netherlands</v>
+      </c>
+      <c r="I9" s="7" t="e">
+        <f>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J9" s="1" t="e">
+        <f>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K9" s="8" t="str">
+        <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
+_xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
+        <v>'GNFR-NFR'!C2:C128</v>
+      </c>
+      <c r="L9" s="3" t="e">
+        <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M9" s="8">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
+        <v>2005</v>
+      </c>
+      <c r="N9" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[emission_type]]),"",tbl_I_scaling[[#This Row],[emission_type]])</f>
+        <v>*</v>
+      </c>
+      <c r="O9" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[pollutant_code]]),"",tbl_I_scaling[[#This Row],[pollutant_code]])</f>
+        <v>Cd</v>
+      </c>
+      <c r="P9" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[country_iso_code]]),"",tbl_I_scaling[[#This Row],[country_iso_code]])</f>
+        <v>NL</v>
+      </c>
+      <c r="Q9" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_scaling[[#This Row],[GNFR_code]])</f>
+        <v>*</v>
+      </c>
+      <c r="R9" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[NFR_code]]),"*",tbl_I_scaling[[#This Row],[NFR_code]])</f>
+        <v>*</v>
+      </c>
+      <c r="S9" s="8">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[scale_factor]]),"",tbl_I_scaling[[#This Row],[scale_factor]])</f>
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="F2:F8">
-    <cfRule type="expression" dxfId="18" priority="8">
+  <conditionalFormatting sqref="F2:F9">
+    <cfRule type="expression" dxfId="16" priority="8">
       <formula>$L2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G8 A2:D8">
-    <cfRule type="expression" dxfId="17" priority="7">
+  <conditionalFormatting sqref="G2:G9 A2:D9">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>ISBLANK(A2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8" xr:uid="{C611A4C6-CA77-4AE0-BA3A-386AF40032A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9" xr:uid="{C611A4C6-CA77-4AE0-BA3A-386AF40032A9}">
       <formula1>emission_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C8" xr:uid="{81D70F75-C546-4EC8-8B25-35F3C22201A8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{81D70F75-C546-4EC8-8B25-35F3C22201A8}">
       <formula1>pollutant</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8" xr:uid="{B9574AEF-5AB3-408B-8C01-0C834356DBF3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9" xr:uid="{B9574AEF-5AB3-408B-8C01-0C834356DBF3}">
       <formula1>country</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F8" xr:uid="{B436CDB6-B312-4604-8DD0-70B496D01FA8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{B436CDB6-B312-4604-8DD0-70B496D01FA8}">
       <formula1>INDIRECT(K2)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Improved scaling factor wildcard prioritization
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/02_scaling/scaling.xlsx
+++ b/logic/test/data/_input/02_scaling/scaling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\_input\02_scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63CB0CE2-7CD4-46D6-814C-CF858DBDDD7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FAC542-A64E-4001-99BC-01D53966C024}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="6" xr2:uid="{6C3FE3BB-8C73-4241-95BD-F737EA4A19F7}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="447">
   <si>
     <t>A_PublicPower</t>
   </si>
@@ -1833,8 +1833,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6617CD5-2290-43AE-9640-6C7136C3D81F}" name="tbl_I_scaling" displayName="tbl_I_scaling" ref="A1:S9" totalsRowShown="0">
-  <autoFilter ref="A1:S9" xr:uid="{63E30767-0150-412D-B197-11CE9D14EB4E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6617CD5-2290-43AE-9640-6C7136C3D81F}" name="tbl_I_scaling" displayName="tbl_I_scaling" ref="A1:S10" totalsRowShown="0">
+  <autoFilter ref="A1:S10" xr:uid="{63E30767-0150-412D-B197-11CE9D14EB4E}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{3CCF1BDF-57B8-4181-91EA-C6A954F57C6F}" name="year" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{85345B25-FBFE-4C64-BB97-93F81600465B}" name="emission_type"/>
@@ -5001,10 +5001,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5624,29 +5624,98 @@
         <v>0.8</v>
       </c>
     </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>2005</v>
+      </c>
+      <c r="B10" t="s">
+        <v>444</v>
+      </c>
+      <c r="C10" t="s">
+        <v>407</v>
+      </c>
+      <c r="D10" t="s">
+        <v>369</v>
+      </c>
+      <c r="F10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10">
+        <v>0.5</v>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f>INDEX(tbl_country[country_label],MATCH(tbl_I_scaling[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</f>
+        <v>Netherlands</v>
+      </c>
+      <c r="I10" s="7" t="str">
+        <f>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
+        <v>E_Solvents</v>
+      </c>
+      <c r="J10" s="1" t="str">
+        <f>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
+        <v>Coating applications</v>
+      </c>
+      <c r="K10" s="8" t="str">
+        <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
+_xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
+        <v>'GNFR-NFR'!C2:C128</v>
+      </c>
+      <c r="L10" s="3" t="b">
+        <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
+        <v>0</v>
+      </c>
+      <c r="M10" s="8">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
+        <v>2005</v>
+      </c>
+      <c r="N10" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[emission_type]]),"",tbl_I_scaling[[#This Row],[emission_type]])</f>
+        <v>*</v>
+      </c>
+      <c r="O10" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[pollutant_code]]),"",tbl_I_scaling[[#This Row],[pollutant_code]])</f>
+        <v>Cd</v>
+      </c>
+      <c r="P10" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[country_iso_code]]),"",tbl_I_scaling[[#This Row],[country_iso_code]])</f>
+        <v>NL</v>
+      </c>
+      <c r="Q10" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_scaling[[#This Row],[GNFR_code]])</f>
+        <v>E</v>
+      </c>
+      <c r="R10" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[NFR_code]]),"*",tbl_I_scaling[[#This Row],[NFR_code]])</f>
+        <v>2D3d</v>
+      </c>
+      <c r="S10" s="8">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[scale_factor]]),"",tbl_I_scaling[[#This Row],[scale_factor]])</f>
+        <v>0.5</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="F2:F9">
+  <conditionalFormatting sqref="F2:F10">
     <cfRule type="expression" dxfId="16" priority="8">
       <formula>$L2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G9 A2:D9">
+  <conditionalFormatting sqref="G2:G10 A2:D10">
     <cfRule type="expression" dxfId="15" priority="7">
       <formula>ISBLANK(A2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B9" xr:uid="{C611A4C6-CA77-4AE0-BA3A-386AF40032A9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{C611A4C6-CA77-4AE0-BA3A-386AF40032A9}">
       <formula1>emission_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{81D70F75-C546-4EC8-8B25-35F3C22201A8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{81D70F75-C546-4EC8-8B25-35F3C22201A8}">
       <formula1>pollutant</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9" xr:uid="{B9574AEF-5AB3-408B-8C01-0C834356DBF3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10" xr:uid="{B9574AEF-5AB3-408B-8C01-0C834356DBF3}">
       <formula1>country</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{B436CDB6-B312-4604-8DD0-70B496D01FA8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{B436CDB6-B312-4604-8DD0-70B496D01FA8}">
       <formula1>INDIRECT(K2)</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Scaling factors path can be configured. Use first match from the file instead of scoring system
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/02_scaling/scaling.xlsx
+++ b/logic/test/data/_input/02_scaling/scaling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\_input\02_scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FAC542-A64E-4001-99BC-01D53966C024}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EC98BE-A81B-4F5F-B1F9-67FB1BA3089E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="6" xr2:uid="{6C3FE3BB-8C73-4241-95BD-F737EA4A19F7}"/>
+    <workbookView xWindow="-23148" yWindow="11184" windowWidth="23256" windowHeight="14616" activeTab="6" xr2:uid="{6C3FE3BB-8C73-4241-95BD-F737EA4A19F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Emission type" sheetId="5" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="447">
   <si>
     <t>A_PublicPower</t>
   </si>
@@ -1535,7 +1535,37 @@
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1736,26 +1766,6 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1833,51 +1843,51 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6617CD5-2290-43AE-9640-6C7136C3D81F}" name="tbl_I_scaling" displayName="tbl_I_scaling" ref="A1:S10" totalsRowShown="0">
-  <autoFilter ref="A1:S10" xr:uid="{63E30767-0150-412D-B197-11CE9D14EB4E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6617CD5-2290-43AE-9640-6C7136C3D81F}" name="tbl_I_scaling" displayName="tbl_I_scaling" ref="A1:S11" totalsRowShown="0">
+  <autoFilter ref="A1:S11" xr:uid="{63E30767-0150-412D-B197-11CE9D14EB4E}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{3CCF1BDF-57B8-4181-91EA-C6A954F57C6F}" name="year" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{3CCF1BDF-57B8-4181-91EA-C6A954F57C6F}" name="year" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{85345B25-FBFE-4C64-BB97-93F81600465B}" name="emission_type"/>
     <tableColumn id="3" xr3:uid="{E47F6DBE-843D-4D02-9E5B-FEE4182373E7}" name="pollutant_code"/>
     <tableColumn id="8" xr3:uid="{E38CAB6A-CB47-4542-997D-36BA98FB4911}" name="country_iso_code"/>
     <tableColumn id="4" xr3:uid="{98A5C858-28E9-44AB-8218-0A98439E4FDD}" name="GNFR_code"/>
     <tableColumn id="5" xr3:uid="{E012C600-87B4-47D1-9988-30D2C112D83D}" name="NFR_code"/>
     <tableColumn id="12" xr3:uid="{2155F8C1-A823-4717-B464-22F4A9A05E6A}" name="scale_factor"/>
-    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="13">
+    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="16">
       <calculatedColumnFormula>INDEX(tbl_country[country_label],MATCH(tbl_I_scaling[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="15">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="14">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="10">
+    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="13">
       <calculatedColumnFormula>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="9">
+    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="12">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="8">
+    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="11">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{F0E4C9D2-7F88-4B77-907E-74002F493346}" name="E-MAP_emission_type" dataDxfId="7">
+    <tableColumn id="14" xr3:uid="{F0E4C9D2-7F88-4B77-907E-74002F493346}" name="E-MAP_emission_type" dataDxfId="10">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[emission_type]]),"",tbl_I_scaling[[#This Row],[emission_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="6">
+    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="9">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[pollutant_code]]),"",tbl_I_scaling[[#This Row],[pollutant_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="5">
+    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="8">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[country_iso_code]]),"",tbl_I_scaling[[#This Row],[country_iso_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="4">
+    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="7">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_scaling[[#This Row],[GNFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="3">
+    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[NFR_code]]),"*",tbl_I_scaling[[#This Row],[NFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_scale_factor" dataDxfId="2">
+    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_scale_factor" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[scale_factor]]),"",tbl_I_scaling[[#This Row],[scale_factor]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2199,22 +2209,22 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>425</v>
       </c>
@@ -2238,13 +2248,13 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -2252,7 +2262,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -2260,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -2268,7 +2278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -2276,7 +2286,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>147</v>
       </c>
@@ -2284,7 +2294,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>148</v>
       </c>
@@ -2292,7 +2302,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -2300,7 +2310,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -2308,7 +2318,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -2316,7 +2326,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>152</v>
       </c>
@@ -2324,7 +2334,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -2332,7 +2342,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>154</v>
       </c>
@@ -2340,7 +2350,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -2348,7 +2358,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>156</v>
       </c>
@@ -2375,15 +2385,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="109.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="109.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -2397,7 +2407,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -2412,7 +2422,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -2427,7 +2437,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -2442,7 +2452,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -2457,7 +2467,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>145</v>
       </c>
@@ -2472,7 +2482,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -2487,7 +2497,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -2502,7 +2512,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>145</v>
       </c>
@@ -2517,7 +2527,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>145</v>
       </c>
@@ -2532,7 +2542,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -2547,7 +2557,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -2562,7 +2572,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>145</v>
       </c>
@@ -2577,7 +2587,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -2592,7 +2602,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>145</v>
       </c>
@@ -2607,7 +2617,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>145</v>
       </c>
@@ -2622,7 +2632,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -2637,7 +2647,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -2652,7 +2662,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -2667,7 +2677,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>145</v>
       </c>
@@ -2682,7 +2692,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -2697,7 +2707,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -2712,7 +2722,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -2727,7 +2737,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>145</v>
       </c>
@@ -2742,7 +2752,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>145</v>
       </c>
@@ -2757,7 +2767,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>145</v>
       </c>
@@ -2772,7 +2782,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -2787,7 +2797,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>145</v>
       </c>
@@ -2802,7 +2812,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>145</v>
       </c>
@@ -2817,7 +2827,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>145</v>
       </c>
@@ -2832,7 +2842,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -2847,7 +2857,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -2862,7 +2872,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -2877,7 +2887,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -2892,7 +2902,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>145</v>
       </c>
@@ -2907,7 +2917,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>145</v>
       </c>
@@ -2922,7 +2932,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>145</v>
       </c>
@@ -2937,7 +2947,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -2952,7 +2962,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>145</v>
       </c>
@@ -2967,7 +2977,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -2982,7 +2992,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>145</v>
       </c>
@@ -2997,7 +3007,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>145</v>
       </c>
@@ -3012,7 +3022,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -3027,7 +3037,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>145</v>
       </c>
@@ -3042,7 +3052,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>145</v>
       </c>
@@ -3057,7 +3067,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>146</v>
       </c>
@@ -3072,7 +3082,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>146</v>
       </c>
@@ -3087,7 +3097,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>146</v>
       </c>
@@ -3102,7 +3112,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -3117,7 +3127,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>147</v>
       </c>
@@ -3132,7 +3142,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>147</v>
       </c>
@@ -3147,7 +3157,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -3162,7 +3172,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -3177,7 +3187,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>147</v>
       </c>
@@ -3192,7 +3202,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>147</v>
       </c>
@@ -3207,7 +3217,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>147</v>
       </c>
@@ -3222,7 +3232,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>147</v>
       </c>
@@ -3237,7 +3247,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>147</v>
       </c>
@@ -3252,7 +3262,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>148</v>
       </c>
@@ -3267,7 +3277,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>148</v>
       </c>
@@ -3282,7 +3292,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>148</v>
       </c>
@@ -3297,7 +3307,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>148</v>
       </c>
@@ -3312,7 +3322,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>148</v>
       </c>
@@ -3327,7 +3337,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>148</v>
       </c>
@@ -3342,7 +3352,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -3357,7 +3367,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -3372,7 +3382,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>149</v>
       </c>
@@ -3387,7 +3397,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>149</v>
       </c>
@@ -3402,7 +3412,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>149</v>
       </c>
@@ -3417,7 +3427,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>149</v>
       </c>
@@ -3432,7 +3442,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -3447,7 +3457,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>149</v>
       </c>
@@ -3462,7 +3472,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -3477,7 +3487,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>150</v>
       </c>
@@ -3492,7 +3502,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -3507,7 +3517,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>151</v>
       </c>
@@ -3522,7 +3532,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>151</v>
       </c>
@@ -3537,7 +3547,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -3552,7 +3562,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>152</v>
       </c>
@@ -3567,7 +3577,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>152</v>
       </c>
@@ -3582,7 +3592,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>152</v>
       </c>
@@ -3597,7 +3607,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>152</v>
       </c>
@@ -3612,7 +3622,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>152</v>
       </c>
@@ -3627,7 +3637,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>152</v>
       </c>
@@ -3642,7 +3652,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>152</v>
       </c>
@@ -3657,7 +3667,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>152</v>
       </c>
@@ -3672,7 +3682,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>153</v>
       </c>
@@ -3687,7 +3697,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>153</v>
       </c>
@@ -3702,7 +3712,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>153</v>
       </c>
@@ -3717,7 +3727,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>153</v>
       </c>
@@ -3732,7 +3742,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>153</v>
       </c>
@@ -3747,7 +3757,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>153</v>
       </c>
@@ -3762,7 +3772,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>153</v>
       </c>
@@ -3777,7 +3787,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -3792,7 +3802,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>153</v>
       </c>
@@ -3807,7 +3817,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>153</v>
       </c>
@@ -3822,7 +3832,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>153</v>
       </c>
@@ -3837,7 +3847,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>153</v>
       </c>
@@ -3852,7 +3862,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>153</v>
       </c>
@@ -3867,7 +3877,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>153</v>
       </c>
@@ -3882,7 +3892,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>153</v>
       </c>
@@ -3897,7 +3907,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>154</v>
       </c>
@@ -3912,7 +3922,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>154</v>
       </c>
@@ -3927,7 +3937,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>154</v>
       </c>
@@ -3942,7 +3952,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>154</v>
       </c>
@@ -3957,7 +3967,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>154</v>
       </c>
@@ -3972,7 +3982,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>154</v>
       </c>
@@ -3987,7 +3997,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>154</v>
       </c>
@@ -4002,7 +4012,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>154</v>
       </c>
@@ -4017,7 +4027,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>154</v>
       </c>
@@ -4032,7 +4042,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>154</v>
       </c>
@@ -4047,7 +4057,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>154</v>
       </c>
@@ -4062,7 +4072,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>154</v>
       </c>
@@ -4077,7 +4087,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>154</v>
       </c>
@@ -4092,7 +4102,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>155</v>
       </c>
@@ -4107,7 +4117,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>155</v>
       </c>
@@ -4122,7 +4132,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>155</v>
       </c>
@@ -4137,7 +4147,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>155</v>
       </c>
@@ -4152,7 +4162,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>155</v>
       </c>
@@ -4167,7 +4177,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>155</v>
       </c>
@@ -4182,7 +4192,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>155</v>
       </c>
@@ -4197,7 +4207,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>155</v>
       </c>
@@ -4212,7 +4222,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>155</v>
       </c>
@@ -4227,7 +4237,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>155</v>
       </c>
@@ -4242,7 +4252,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>155</v>
       </c>
@@ -4257,7 +4267,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>155</v>
       </c>
@@ -4272,7 +4282,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>155</v>
       </c>
@@ -4287,7 +4297,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>156</v>
       </c>
@@ -4321,13 +4331,13 @@
       <selection activeCell="A2" sqref="A2:A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>284</v>
       </c>
@@ -4335,7 +4345,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>285</v>
       </c>
@@ -4343,7 +4353,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>287</v>
       </c>
@@ -4351,7 +4361,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -4359,7 +4369,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>291</v>
       </c>
@@ -4367,7 +4377,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>293</v>
       </c>
@@ -4375,7 +4385,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>295</v>
       </c>
@@ -4383,7 +4393,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>297</v>
       </c>
@@ -4391,7 +4401,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>299</v>
       </c>
@@ -4399,7 +4409,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>301</v>
       </c>
@@ -4407,7 +4417,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>303</v>
       </c>
@@ -4415,7 +4425,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>305</v>
       </c>
@@ -4423,7 +4433,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>307</v>
       </c>
@@ -4431,7 +4441,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>309</v>
       </c>
@@ -4439,7 +4449,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>311</v>
       </c>
@@ -4447,7 +4457,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>313</v>
       </c>
@@ -4455,7 +4465,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>315</v>
       </c>
@@ -4463,7 +4473,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>317</v>
       </c>
@@ -4471,7 +4481,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>319</v>
       </c>
@@ -4479,7 +4489,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>321</v>
       </c>
@@ -4487,7 +4497,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>323</v>
       </c>
@@ -4495,7 +4505,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>325</v>
       </c>
@@ -4503,7 +4513,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>327</v>
       </c>
@@ -4511,7 +4521,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>329</v>
       </c>
@@ -4519,7 +4529,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>331</v>
       </c>
@@ -4527,7 +4537,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>333</v>
       </c>
@@ -4535,7 +4545,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>335</v>
       </c>
@@ -4543,7 +4553,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>337</v>
       </c>
@@ -4551,7 +4561,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>339</v>
       </c>
@@ -4559,7 +4569,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>341</v>
       </c>
@@ -4567,7 +4577,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>343</v>
       </c>
@@ -4575,7 +4585,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>345</v>
       </c>
@@ -4583,7 +4593,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>347</v>
       </c>
@@ -4591,7 +4601,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>349</v>
       </c>
@@ -4599,7 +4609,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>351</v>
       </c>
@@ -4607,7 +4617,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>353</v>
       </c>
@@ -4615,7 +4625,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>355</v>
       </c>
@@ -4623,7 +4633,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>357</v>
       </c>
@@ -4631,7 +4641,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>359</v>
       </c>
@@ -4639,7 +4649,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>361</v>
       </c>
@@ -4647,7 +4657,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>363</v>
       </c>
@@ -4655,7 +4665,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>365</v>
       </c>
@@ -4663,7 +4673,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>367</v>
       </c>
@@ -4671,7 +4681,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>369</v>
       </c>
@@ -4679,7 +4689,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>371</v>
       </c>
@@ -4687,7 +4697,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>373</v>
       </c>
@@ -4695,7 +4705,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>375</v>
       </c>
@@ -4703,7 +4713,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>377</v>
       </c>
@@ -4711,7 +4721,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>379</v>
       </c>
@@ -4719,7 +4729,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>381</v>
       </c>
@@ -4727,7 +4737,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>383</v>
       </c>
@@ -4735,7 +4745,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>385</v>
       </c>
@@ -4743,7 +4753,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>387</v>
       </c>
@@ -4751,7 +4761,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>389</v>
       </c>
@@ -4759,7 +4769,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>391</v>
       </c>
@@ -4767,7 +4777,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>393</v>
       </c>
@@ -4794,147 +4804,147 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>422</v>
       </c>
@@ -4958,9 +4968,9 @@
       <selection activeCell="C6" sqref="C6:L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>435</v>
       </c>
@@ -4971,22 +4981,22 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>438</v>
       </c>
@@ -5001,19 +5011,19 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="9"/>
-    <col min="11" max="12" width="22.42578125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" style="9"/>
+    <col min="11" max="12" width="22.453125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>441</v>
       </c>
@@ -5072,9 +5082,9 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
-        <v>444</v>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="9">
+        <v>2015</v>
       </c>
       <c r="B2" t="s">
         <v>424</v>
@@ -5112,9 +5122,9 @@
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
         <v>0</v>
       </c>
-      <c r="M2" s="3" t="str">
+      <c r="M2" s="3">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
-        <v>*</v>
+        <v>2015</v>
       </c>
       <c r="N2" s="3" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[emission_type]]),"",tbl_I_scaling[[#This Row],[emission_type]])</f>
@@ -5141,9 +5151,9 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="9">
-        <v>2015</v>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>444</v>
       </c>
       <c r="B3" t="s">
         <v>424</v>
@@ -5181,9 +5191,9 @@
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
         <v>0</v>
       </c>
-      <c r="M3" s="8">
+      <c r="M3" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
-        <v>2015</v>
+        <v>*</v>
       </c>
       <c r="N3" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[emission_type]]),"",tbl_I_scaling[[#This Row],[emission_type]])</f>
@@ -5210,7 +5220,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <v>2015</v>
       </c>
@@ -5279,7 +5289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>445</v>
       </c>
@@ -5348,7 +5358,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="9">
         <v>2015</v>
       </c>
@@ -5417,7 +5427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>445</v>
       </c>
@@ -5486,7 +5496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>446</v>
       </c>
@@ -5555,49 +5565,49 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
-        <v>2005</v>
+        <v>2000</v>
       </c>
       <c r="B9" t="s">
         <v>444</v>
       </c>
       <c r="C9" t="s">
-        <v>407</v>
+        <v>444</v>
       </c>
       <c r="D9" t="s">
-        <v>369</v>
-      </c>
-      <c r="E9" t="s">
         <v>444</v>
       </c>
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
       <c r="G9">
-        <v>0.8</v>
+        <v>10</v>
       </c>
       <c r="H9" s="1" t="str">
         <f>INDEX(tbl_country[country_label],MATCH(tbl_I_scaling[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</f>
-        <v>Netherlands</v>
-      </c>
-      <c r="I9" s="7" t="e">
+        <v>Albania</v>
+      </c>
+      <c r="I9" s="7" t="str">
         <f>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J9" s="1" t="e">
+        <v>J_Waste</v>
+      </c>
+      <c r="J9" s="1" t="str">
         <f>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
-        <v>#N/A</v>
+        <v>Other waste (please specify in the IIR)</v>
       </c>
       <c r="K9" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
         <v>'GNFR-NFR'!C2:C128</v>
       </c>
-      <c r="L9" s="3" t="e">
+      <c r="L9" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="M9" s="8">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
-        <v>2005</v>
+        <v>2000</v>
       </c>
       <c r="N9" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[emission_type]]),"",tbl_I_scaling[[#This Row],[emission_type]])</f>
@@ -5605,26 +5615,26 @@
       </c>
       <c r="O9" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[pollutant_code]]),"",tbl_I_scaling[[#This Row],[pollutant_code]])</f>
-        <v>Cd</v>
+        <v>*</v>
       </c>
       <c r="P9" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[country_iso_code]]),"",tbl_I_scaling[[#This Row],[country_iso_code]])</f>
-        <v>NL</v>
+        <v>*</v>
       </c>
       <c r="Q9" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_scaling[[#This Row],[GNFR_code]])</f>
-        <v>*</v>
+        <v>J</v>
       </c>
       <c r="R9" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[NFR_code]]),"*",tbl_I_scaling[[#This Row],[NFR_code]])</f>
-        <v>*</v>
+        <v>5E</v>
       </c>
       <c r="S9" s="8">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[scale_factor]]),"",tbl_I_scaling[[#This Row],[scale_factor]])</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <v>2005</v>
       </c>
@@ -5693,30 +5703,120 @@
         <v>0.5</v>
       </c>
     </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>2005</v>
+      </c>
+      <c r="B11" t="s">
+        <v>444</v>
+      </c>
+      <c r="C11" t="s">
+        <v>407</v>
+      </c>
+      <c r="D11" t="s">
+        <v>369</v>
+      </c>
+      <c r="E11" t="s">
+        <v>444</v>
+      </c>
+      <c r="G11">
+        <v>0.8</v>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f>INDEX(tbl_country[country_label],MATCH(tbl_I_scaling[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</f>
+        <v>Netherlands</v>
+      </c>
+      <c r="I11" s="7" t="e">
+        <f>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="J11" s="1" t="e">
+        <f>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="K11" s="8" t="str">
+        <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
+_xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
+        <v>'GNFR-NFR'!C2:C128</v>
+      </c>
+      <c r="L11" s="3" t="e">
+        <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M11" s="8">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
+        <v>2005</v>
+      </c>
+      <c r="N11" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[emission_type]]),"",tbl_I_scaling[[#This Row],[emission_type]])</f>
+        <v>*</v>
+      </c>
+      <c r="O11" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[pollutant_code]]),"",tbl_I_scaling[[#This Row],[pollutant_code]])</f>
+        <v>Cd</v>
+      </c>
+      <c r="P11" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[country_iso_code]]),"",tbl_I_scaling[[#This Row],[country_iso_code]])</f>
+        <v>NL</v>
+      </c>
+      <c r="Q11" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_scaling[[#This Row],[GNFR_code]])</f>
+        <v>*</v>
+      </c>
+      <c r="R11" s="8" t="str">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[NFR_code]]),"*",tbl_I_scaling[[#This Row],[NFR_code]])</f>
+        <v>*</v>
+      </c>
+      <c r="S11" s="8">
+        <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[scale_factor]]),"",tbl_I_scaling[[#This Row],[scale_factor]])</f>
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="F2:F10">
-    <cfRule type="expression" dxfId="16" priority="8">
+  <conditionalFormatting sqref="F2:F8">
+    <cfRule type="expression" dxfId="4" priority="11">
       <formula>$L2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G10 A2:D10">
-    <cfRule type="expression" dxfId="15" priority="7">
+  <conditionalFormatting sqref="G2:G8 G10:G11 A2:D8 A10:D11">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>ISBLANK(A2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B10" xr:uid="{C611A4C6-CA77-4AE0-BA3A-386AF40032A9}">
+  <conditionalFormatting sqref="F11">
+    <cfRule type="expression" dxfId="2" priority="13">
+      <formula>$L9=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$L9=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="expression" dxfId="0" priority="14">
+      <formula>#REF!=FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B8 B10:B11" xr:uid="{E91CBEAB-428A-4E75-9614-430CE89F7C46}">
       <formula1>emission_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10" xr:uid="{81D70F75-C546-4EC8-8B25-35F3C22201A8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C8 C10:C11" xr:uid="{31A25EC4-B55C-4BEF-A211-C3848E466A10}">
       <formula1>pollutant</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10" xr:uid="{B9574AEF-5AB3-408B-8C01-0C834356DBF3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8 D10:D11" xr:uid="{3E37EA03-142B-4C7D-B458-082339088B9D}">
       <formula1>country</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{B436CDB6-B312-4604-8DD0-70B496D01FA8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{CE2DE840-8711-490D-9E3B-300483CF5759}">
       <formula1>INDIRECT(K2)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10" xr:uid="{4ACF885D-5B4F-4B20-A764-168724063246}">
+      <formula1>INDIRECT(#REF!)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F11" xr:uid="{5A50A710-9916-4CE8-BBB2-73905CC2DFE5}">
+      <formula1>INDIRECT(K9)</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Scaling template update. Nfr and Gnfr entries are required
</commit_message>
<xml_diff>
--- a/logic/test/data/_input/02_scaling/scaling.xlsx
+++ b/logic/test/data/_input/02_scaling/scaling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RMABuild\emap\logic\test\data\_input\02_scaling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66EC98BE-A81B-4F5F-B1F9-67FB1BA3089E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE9A823-F9F8-45B6-9C5D-9E36311F0F33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="11184" windowWidth="23256" windowHeight="14616" activeTab="6" xr2:uid="{6C3FE3BB-8C73-4241-95BD-F737EA4A19F7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="6" xr2:uid="{6C3FE3BB-8C73-4241-95BD-F737EA4A19F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Emission type" sheetId="5" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="447">
   <si>
     <t>A_PublicPower</t>
   </si>
@@ -1536,56 +1536,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1766,6 +1716,56 @@
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1846,48 +1846,48 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C6617CD5-2290-43AE-9640-6C7136C3D81F}" name="tbl_I_scaling" displayName="tbl_I_scaling" ref="A1:S11" totalsRowShown="0">
   <autoFilter ref="A1:S11" xr:uid="{63E30767-0150-412D-B197-11CE9D14EB4E}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{3CCF1BDF-57B8-4181-91EA-C6A954F57C6F}" name="year" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{3CCF1BDF-57B8-4181-91EA-C6A954F57C6F}" name="year" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{85345B25-FBFE-4C64-BB97-93F81600465B}" name="emission_type"/>
     <tableColumn id="3" xr3:uid="{E47F6DBE-843D-4D02-9E5B-FEE4182373E7}" name="pollutant_code"/>
     <tableColumn id="8" xr3:uid="{E38CAB6A-CB47-4542-997D-36BA98FB4911}" name="country_iso_code"/>
     <tableColumn id="4" xr3:uid="{98A5C858-28E9-44AB-8218-0A98439E4FDD}" name="GNFR_code"/>
     <tableColumn id="5" xr3:uid="{E012C600-87B4-47D1-9988-30D2C112D83D}" name="NFR_code"/>
     <tableColumn id="12" xr3:uid="{2155F8C1-A823-4717-B464-22F4A9A05E6A}" name="scale_factor"/>
-    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="16">
+    <tableColumn id="9" xr3:uid="{DCB47D4C-7148-4891-B486-04CF70C7FDCC}" name="country_label" dataDxfId="11">
       <calculatedColumnFormula>INDEX(tbl_country[country_label],MATCH(tbl_I_scaling[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="15">
+    <tableColumn id="6" xr3:uid="{409654D3-E717-4ECD-B724-CE76BF1FA726}" name="GNFR_label" dataDxfId="10">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="14">
+    <tableColumn id="7" xr3:uid="{B9A37C5B-FED3-493F-81B8-F88D72CF166B}" name="NFR_label" dataDxfId="9">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="13">
+    <tableColumn id="10" xr3:uid="{3741CCE9-D8A3-4702-9FBB-BDDC5296CA41}" name="Data validation GNFR-NFR_range" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="12">
+    <tableColumn id="11" xr3:uid="{327D5723-70F8-4F14-A112-90BAA56B122D}" name="Data validation GNFR-NFR_ok" dataDxfId="7">
       <calculatedColumnFormula>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="11">
+    <tableColumn id="13" xr3:uid="{14DFCA77-FA4F-4492-90FC-E1CF29BD5BDC}" name="E-MAP_year" dataDxfId="6">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{F0E4C9D2-7F88-4B77-907E-74002F493346}" name="E-MAP_emission_type" dataDxfId="10">
+    <tableColumn id="14" xr3:uid="{F0E4C9D2-7F88-4B77-907E-74002F493346}" name="E-MAP_emission_type" dataDxfId="5">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[emission_type]]),"",tbl_I_scaling[[#This Row],[emission_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="9">
+    <tableColumn id="15" xr3:uid="{0AF0B6B0-EAF2-4779-805E-3E840BA3636B}" name="E-MAP_pollutant_code" dataDxfId="4">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[pollutant_code]]),"",tbl_I_scaling[[#This Row],[pollutant_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="8">
+    <tableColumn id="16" xr3:uid="{C9437DA3-379A-4119-852E-97451565DC30}" name="E-MAP_country_iso_code" dataDxfId="3">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[country_iso_code]]),"",tbl_I_scaling[[#This Row],[country_iso_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="7">
+    <tableColumn id="17" xr3:uid="{90BD55C3-62EC-45E1-88D6-C55C69ABA3CE}" name="E-MAP_GNFR_code" dataDxfId="2">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[GNFR_code]]),INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0)),tbl_I_scaling[[#This Row],[GNFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="6">
+    <tableColumn id="18" xr3:uid="{75A83B3D-980A-4F01-8C60-1E833397AAFE}" name="E-MAP_NFR_code" dataDxfId="1">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[NFR_code]]),"*",tbl_I_scaling[[#This Row],[NFR_code]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_scale_factor" dataDxfId="5">
+    <tableColumn id="19" xr3:uid="{8B2B56DD-9D26-4198-95A5-38E1BF66DD11}" name="E-MAP_scale_factor" dataDxfId="0">
       <calculatedColumnFormula>IF(ISBLANK(tbl_I_scaling[[#This Row],[scale_factor]]),"",tbl_I_scaling[[#This Row],[scale_factor]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2209,22 +2209,22 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>425</v>
       </c>
@@ -2248,13 +2248,13 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>147</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>148</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>151</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>152</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>154</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>156</v>
       </c>
@@ -2385,15 +2385,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.81640625" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.77734375" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="109.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="109.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>143</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -2437,7 +2437,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>145</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>145</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>145</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>145</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>145</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>145</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>145</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>145</v>
       </c>
@@ -2587,7 +2587,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>145</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>145</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>145</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>145</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>145</v>
       </c>
@@ -2707,7 +2707,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>145</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>145</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>145</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>145</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>145</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>145</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>145</v>
       </c>
@@ -2827,7 +2827,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>145</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>145</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>145</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>145</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>145</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>145</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>145</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>145</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>145</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>145</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>145</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>145</v>
       </c>
@@ -3052,7 +3052,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>145</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>146</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>146</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>146</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>146</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>147</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>147</v>
       </c>
@@ -3157,7 +3157,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>147</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -3187,7 +3187,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>147</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>147</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>147</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>147</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>147</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>148</v>
       </c>
@@ -3277,7 +3277,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>148</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>148</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>148</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>148</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>148</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>148</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>149</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>149</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>149</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>149</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>149</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>150</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>151</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>151</v>
       </c>
@@ -3547,7 +3547,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>152</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>152</v>
       </c>
@@ -3577,7 +3577,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>152</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>152</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>152</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>152</v>
       </c>
@@ -3637,7 +3637,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>152</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>152</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>152</v>
       </c>
@@ -3682,7 +3682,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>153</v>
       </c>
@@ -3697,7 +3697,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>153</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>153</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>153</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>153</v>
       </c>
@@ -3757,7 +3757,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>153</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>153</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>153</v>
       </c>
@@ -3817,7 +3817,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>153</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>153</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>153</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>153</v>
       </c>
@@ -3877,7 +3877,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>153</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>153</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>154</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>154</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>154</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>154</v>
       </c>
@@ -3967,7 +3967,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>154</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>154</v>
       </c>
@@ -3997,7 +3997,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>154</v>
       </c>
@@ -4012,7 +4012,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>154</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>154</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>154</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>154</v>
       </c>
@@ -4072,7 +4072,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>154</v>
       </c>
@@ -4087,7 +4087,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>154</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>155</v>
       </c>
@@ -4117,7 +4117,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>155</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>155</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>155</v>
       </c>
@@ -4162,7 +4162,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>155</v>
       </c>
@@ -4177,7 +4177,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>155</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>155</v>
       </c>
@@ -4207,7 +4207,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>155</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>155</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>155</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>155</v>
       </c>
@@ -4267,7 +4267,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>155</v>
       </c>
@@ -4282,7 +4282,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>155</v>
       </c>
@@ -4297,7 +4297,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>156</v>
       </c>
@@ -4331,13 +4331,13 @@
       <selection activeCell="A2" sqref="A2:A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" customWidth="1"/>
-    <col min="2" max="2" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="34.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>284</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>285</v>
       </c>
@@ -4353,7 +4353,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>287</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>291</v>
       </c>
@@ -4377,7 +4377,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>293</v>
       </c>
@@ -4385,7 +4385,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>295</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>297</v>
       </c>
@@ -4401,7 +4401,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>299</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>301</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>303</v>
       </c>
@@ -4425,7 +4425,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>305</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>307</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>309</v>
       </c>
@@ -4449,7 +4449,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>311</v>
       </c>
@@ -4457,7 +4457,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>313</v>
       </c>
@@ -4465,7 +4465,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>315</v>
       </c>
@@ -4473,7 +4473,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>317</v>
       </c>
@@ -4481,7 +4481,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>319</v>
       </c>
@@ -4489,7 +4489,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>321</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>323</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>325</v>
       </c>
@@ -4513,7 +4513,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>327</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>329</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>331</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>333</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>335</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>337</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>339</v>
       </c>
@@ -4569,7 +4569,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>341</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>343</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>345</v>
       </c>
@@ -4593,7 +4593,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>347</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>349</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>351</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>353</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>355</v>
       </c>
@@ -4633,7 +4633,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>357</v>
       </c>
@@ -4641,7 +4641,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>359</v>
       </c>
@@ -4649,7 +4649,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>361</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>363</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>365</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>367</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>369</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>371</v>
       </c>
@@ -4697,7 +4697,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>373</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>375</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>377</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>379</v>
       </c>
@@ -4729,7 +4729,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>381</v>
       </c>
@@ -4737,7 +4737,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>383</v>
       </c>
@@ -4745,7 +4745,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>385</v>
       </c>
@@ -4753,7 +4753,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>387</v>
       </c>
@@ -4761,7 +4761,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>389</v>
       </c>
@@ -4769,7 +4769,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>391</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>393</v>
       </c>
@@ -4804,147 +4804,147 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>422</v>
       </c>
@@ -4968,9 +4968,9 @@
       <selection activeCell="C6" sqref="C6:L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>435</v>
       </c>
@@ -4981,22 +4981,22 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>438</v>
       </c>
@@ -5014,16 +5014,16 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="22.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.453125" style="9"/>
-    <col min="11" max="12" width="22.453125" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.44140625" style="9"/>
+    <col min="11" max="12" width="22.44140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>441</v>
       </c>
@@ -5082,7 +5082,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>2015</v>
       </c>
@@ -5094,6 +5094,9 @@
       </c>
       <c r="D2" t="s">
         <v>301</v>
+      </c>
+      <c r="E2" t="s">
+        <v>145</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -5116,11 +5119,11 @@
       <c r="K2" s="3" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
-        <v>'GNFR-NFR'!C2:C128</v>
+        <v>'GNFR-NFR'!C3:C45</v>
       </c>
       <c r="L2" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2" s="3">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5151,7 +5154,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>444</v>
       </c>
@@ -5163,6 +5166,9 @@
       </c>
       <c r="D3" t="s">
         <v>301</v>
+      </c>
+      <c r="E3" t="s">
+        <v>145</v>
       </c>
       <c r="F3" t="s">
         <v>5</v>
@@ -5185,11 +5191,11 @@
       <c r="K3" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
-        <v>'GNFR-NFR'!C2:C128</v>
+        <v>'GNFR-NFR'!C3:C45</v>
       </c>
       <c r="L3" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5220,7 +5226,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>2015</v>
       </c>
@@ -5232,6 +5238,9 @@
       </c>
       <c r="D4" t="s">
         <v>369</v>
+      </c>
+      <c r="E4" t="s">
+        <v>145</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -5254,11 +5263,11 @@
       <c r="K4" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
-        <v>'GNFR-NFR'!C2:C128</v>
+        <v>'GNFR-NFR'!C3:C45</v>
       </c>
       <c r="L4" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4" s="8">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5289,7 +5298,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>445</v>
       </c>
@@ -5301,6 +5310,9 @@
       </c>
       <c r="D5" t="s">
         <v>369</v>
+      </c>
+      <c r="E5" t="s">
+        <v>145</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -5323,11 +5335,11 @@
       <c r="K5" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
-        <v>'GNFR-NFR'!C2:C128</v>
+        <v>'GNFR-NFR'!C3:C45</v>
       </c>
       <c r="L5" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5358,7 +5370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>2015</v>
       </c>
@@ -5373,6 +5385,9 @@
       </c>
       <c r="E6" t="s">
         <v>145</v>
+      </c>
+      <c r="F6" t="s">
+        <v>444</v>
       </c>
       <c r="G6">
         <v>4</v>
@@ -5381,22 +5396,22 @@
         <f>INDEX(tbl_country[country_label],MATCH(tbl_I_scaling[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</f>
         <v>Netherlands</v>
       </c>
-      <c r="I6" s="7" t="e">
+      <c r="I6" s="7" t="str">
         <f>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J6" s="1" t="e">
+        <v>A_PublicPower</v>
+      </c>
+      <c r="J6" s="1" t="str">
         <f>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
-        <v>#N/A</v>
+        <v>Public electricity and heat production</v>
       </c>
       <c r="K6" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
         <v>'GNFR-NFR'!C3:C45</v>
       </c>
-      <c r="L6" s="3" t="e">
+      <c r="L6" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="M6" s="8">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5427,7 +5442,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>445</v>
       </c>
@@ -5439,6 +5454,9 @@
       </c>
       <c r="D7" t="s">
         <v>369</v>
+      </c>
+      <c r="E7" t="s">
+        <v>154</v>
       </c>
       <c r="F7" t="s">
         <v>111</v>
@@ -5461,11 +5479,11 @@
       <c r="K7" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
-        <v>'GNFR-NFR'!C2:C128</v>
+        <v>'GNFR-NFR'!C102:C114</v>
       </c>
       <c r="L7" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5496,7 +5514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>446</v>
       </c>
@@ -5508,6 +5526,9 @@
       </c>
       <c r="D8" t="s">
         <v>369</v>
+      </c>
+      <c r="E8" t="s">
+        <v>154</v>
       </c>
       <c r="F8" t="s">
         <v>111</v>
@@ -5530,11 +5551,11 @@
       <c r="K8" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
-        <v>'GNFR-NFR'!C2:C128</v>
+        <v>'GNFR-NFR'!C102:C114</v>
       </c>
       <c r="L8" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8" s="8" t="str">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5565,7 +5586,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>2000</v>
       </c>
@@ -5577,6 +5598,9 @@
       </c>
       <c r="D9" t="s">
         <v>444</v>
+      </c>
+      <c r="E9" t="s">
+        <v>153</v>
       </c>
       <c r="F9" t="s">
         <v>109</v>
@@ -5599,11 +5623,11 @@
       <c r="K9" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
-        <v>'GNFR-NFR'!C2:C128</v>
+        <v>'GNFR-NFR'!C87:C101</v>
       </c>
       <c r="L9" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="8">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5634,7 +5658,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>2005</v>
       </c>
@@ -5646,6 +5670,9 @@
       </c>
       <c r="D10" t="s">
         <v>369</v>
+      </c>
+      <c r="E10" t="s">
+        <v>148</v>
       </c>
       <c r="F10" t="s">
         <v>63</v>
@@ -5668,11 +5695,11 @@
       <c r="K10" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
-        <v>'GNFR-NFR'!C2:C128</v>
+        <v>'GNFR-NFR'!C59:C66</v>
       </c>
       <c r="L10" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="8">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5703,7 +5730,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>2005</v>
       </c>
@@ -5717,6 +5744,9 @@
         <v>369</v>
       </c>
       <c r="E11" t="s">
+        <v>444</v>
+      </c>
+      <c r="F11" t="s">
         <v>444</v>
       </c>
       <c r="G11">
@@ -5726,22 +5756,22 @@
         <f>INDEX(tbl_country[country_label],MATCH(tbl_I_scaling[[#This Row],[country_iso_code]],tbl_country[country_iso_code],0))</f>
         <v>Netherlands</v>
       </c>
-      <c r="I11" s="7" t="e">
+      <c r="I11" s="7" t="str">
         <f>INDEX(tbl_GNFR_NFR[GNFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J11" s="1" t="e">
+        <v>A_PublicPower</v>
+      </c>
+      <c r="J11" s="1" t="str">
         <f>INDEX(tbl_GNFR_NFR[NFR_label],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))</f>
-        <v>#N/A</v>
+        <v>Public electricity and heat production</v>
       </c>
       <c r="K11" s="8" t="str">
         <f>IFERROR(_xlfn.CONCAT("'GNFR-NFR'!C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],)+1,":C",MATCH(tbl_I_scaling[[#This Row],[GNFR_code]],tbl_GNFR_NFR[GNFR_code],0)+COUNTIF(tbl_GNFR_NFR[GNFR_code],tbl_I_scaling[[#This Row],[GNFR_code]])),
 _xlfn.CONCAT("'GNFR-NFR'!C2:C",COUNTA(tbl_GNFR_NFR[NFR_code])+1))</f>
         <v>'GNFR-NFR'!C2:C128</v>
       </c>
-      <c r="L11" s="3" t="e">
+      <c r="L11" s="3" t="b">
         <f>INDEX(tbl_GNFR_NFR[GNFR_code],MATCH(tbl_I_scaling[[#This Row],[NFR_code]],tbl_GNFR_NFR[NFR_code],0))=tbl_I_scaling[[#This Row],[GNFR_code]]</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="M11" s="8">
         <f>IF(ISBLANK(tbl_I_scaling[[#This Row],[year]]),"",tbl_I_scaling[[#This Row],[year]])</f>
@@ -5775,27 +5805,27 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="F2:F8">
-    <cfRule type="expression" dxfId="4" priority="11">
+    <cfRule type="expression" dxfId="17" priority="11">
       <formula>$L2=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G8 G10:G11 A2:D8 A10:D11">
-    <cfRule type="expression" dxfId="3" priority="10">
+    <cfRule type="expression" dxfId="16" priority="10">
       <formula>ISBLANK(A2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="expression" dxfId="2" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>$L9=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>$L9=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="0" priority="14">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>#REF!=FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>